<commit_message>
Added draaiboek testing files
</commit_message>
<xml_diff>
--- a/demo_projects/slagbomen_project/slagbomen_added_assets.xlsx
+++ b/demo_projects/slagbomen_project/slagbomen_added_assets.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\voorbeeld-case-kokerafsluiting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\PycharmProjects\OTLMOW-GUI\demo_projects\slagbomen_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C667B0-B648-4B3D-A81B-D84B9E0F4EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33B574D-F6E4-4AE4-98C1-F50D61F8AC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ins#Slagboom" sheetId="1" r:id="rId1"/>
     <sheet name="ond#Slagboomarm" sheetId="2" r:id="rId2"/>
     <sheet name="ond#SlagboomarmVerlichting" sheetId="3" r:id="rId3"/>
     <sheet name="ond#Slagboomkolom" sheetId="4" r:id="rId4"/>
-    <sheet name="Keuzelijsten" sheetId="5" r:id="rId5"/>
+    <sheet name="legacy#Kast" sheetId="6" r:id="rId5"/>
+    <sheet name="Keuzelijsten" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="68">
   <si>
     <t>typeURI</t>
   </si>
@@ -219,6 +220,15 @@
   </si>
   <si>
     <t>bareel</t>
+  </si>
+  <si>
+    <t>https://lgc.data.wegenenverkeer.be/ns/installatie#Kast</t>
+  </si>
+  <si>
+    <t>Kast</t>
+  </si>
+  <si>
+    <t>demo_project</t>
   </si>
 </sst>
 </file>
@@ -560,7 +570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -935,6 +945,69 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{250112CD-AB78-4C1B-87C1-5540776F7D49}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="20" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" sqref="J1:K998" xr:uid="{2FD58363-39E4-4B93-87CD-BADA1F81EE91}">
+      <formula1>"TRUE,FALSE,-"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{50CCC19D-78A1-44FE-90AE-0060B6E7891A}">
+          <x14:formula1>
+            <xm:f>Keuzelijsten!$A$2:$A$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>T1:T998</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{E95C0D36-A712-4816-9291-9839B139A539}">
+          <x14:formula1>
+            <xm:f>Keuzelijsten!$B$2:$B$24</xm:f>
+          </x14:formula1>
+          <xm:sqref>O1:O998</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B24"/>
   <sheetViews>

</xml_diff>